<commit_message>
Regular PCB schematic completed. Drafted a poor design for the regulator PCB, then added line voltage safety constraints. Pending PCB redesign.
</commit_message>
<xml_diff>
--- a/speed-controller-parts-brainstorm.xlsx
+++ b/speed-controller-parts-brainstorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/jheath_stanford_edu/Documents/nonsense/sewing/singer4452-speed-controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="927" documentId="8_{CF98681D-D789-4D86-96CC-69D7BE0CF994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC815CBE-7CD5-458D-A50F-9BD26B9596FB}"/>
+  <xr:revisionPtr revIDLastSave="937" documentId="8_{CF98681D-D789-4D86-96CC-69D7BE0CF994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE5D9E57-54E9-449F-BEAC-FF1BEAD60983}"/>
   <bookViews>
-    <workbookView xWindow="18495" yWindow="1095" windowWidth="29760" windowHeight="19035" xr2:uid="{55063511-F0A8-42A5-8409-EFE34AF8E3D6}"/>
+    <workbookView xWindow="18840" yWindow="1440" windowWidth="29760" windowHeight="19035" xr2:uid="{55063511-F0A8-42A5-8409-EFE34AF8E3D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="116">
   <si>
     <t>MFG</t>
   </si>
@@ -370,13 +370,28 @@
   </si>
   <si>
     <t>Digikey #</t>
+  </si>
+  <si>
+    <t>Chassis Box - 1590XX, Diecast, 5.72" x 4.77" x 1.55"</t>
+  </si>
+  <si>
+    <t>Amplified Parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.amplifiedparts.com/products/chassis-box-1590xx-diecast-572-x-477-x-155</t>
+  </si>
+  <si>
+    <t>P-H1590XXCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +449,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -470,7 +491,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -813,7 +834,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +892,6 @@
       <c r="C4" s="10"/>
       <c r="D4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="11"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -883,12 +903,38 @@
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7">
+        <v>12.59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worked out schematic for foot pedal PCB via reverse engineering and LTSpice
</commit_message>
<xml_diff>
--- a/speed-controller-parts-brainstorm.xlsx
+++ b/speed-controller-parts-brainstorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/jheath_stanford_edu/Documents/nonsense/sewing/singer4452-speed-controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="972" documentId="8_{CF98681D-D789-4D86-96CC-69D7BE0CF994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F461E10C-49DA-4048-8910-7399B64595E3}"/>
+  <xr:revisionPtr revIDLastSave="994" documentId="8_{CF98681D-D789-4D86-96CC-69D7BE0CF994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2771B9F-547E-406E-B254-E15119571F8D}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="1365" windowWidth="29760" windowHeight="19035" xr2:uid="{55063511-F0A8-42A5-8409-EFE34AF8E3D6}"/>
+    <workbookView xWindow="16080" yWindow="1935" windowWidth="29760" windowHeight="19035" xr2:uid="{55063511-F0A8-42A5-8409-EFE34AF8E3D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t>MFG</t>
   </si>
@@ -282,9 +282,6 @@
     <t>MFG #</t>
   </si>
   <si>
-    <t>Digikey #</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -292,6 +289,42 @@
   </si>
   <si>
     <t>Potential foot pedal solution:</t>
+  </si>
+  <si>
+    <t>1287-ST</t>
+  </si>
+  <si>
+    <t>(534-1287-ST)</t>
+  </si>
+  <si>
+    <t>Digikey # (Mouser)</t>
+  </si>
+  <si>
+    <t>Terminals PCB STURDI-MNT TERM</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Keystone-Electronics/1287-ST?qs=lQmX4aIt5iBQmFQ9gmrtHw%3D%3D</t>
+  </si>
+  <si>
+    <t>42100-2 (CUT STRIP)</t>
+  </si>
+  <si>
+    <t>(571-421002-CT)</t>
+  </si>
+  <si>
+    <t>Terminals .25 FF REC IS 18-14 Cut Strip of 100</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TE-Connectivity-AMP/42100-2-CUT-STRIP?qs=2FIyTMJ0hNlByrnrD71s6A%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -372,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -385,6 +418,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -727,7 +763,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,13 +781,13 @@
         <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
         <v>79</v>
@@ -773,16 +809,53 @@
       <c r="A2" s="7"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="I4" s="8"/>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -798,7 +871,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -849,7 +922,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added circuit protection, finished foot pedal PCB design, ordered from OSHPark
</commit_message>
<xml_diff>
--- a/speed-controller-parts-brainstorm.xlsx
+++ b/speed-controller-parts-brainstorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/jheath_stanford_edu/Documents/nonsense/sewing/singer4452-speed-controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="994" documentId="8_{CF98681D-D789-4D86-96CC-69D7BE0CF994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2771B9F-547E-406E-B254-E15119571F8D}"/>
+  <xr:revisionPtr revIDLastSave="999" documentId="8_{CF98681D-D789-4D86-96CC-69D7BE0CF994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D047919-799D-40F5-9AE1-FDBA8C275FA6}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="1935" windowWidth="29760" windowHeight="19035" xr2:uid="{55063511-F0A8-42A5-8409-EFE34AF8E3D6}"/>
+    <workbookView xWindow="15375" yWindow="1845" windowWidth="29760" windowHeight="19035" xr2:uid="{55063511-F0A8-42A5-8409-EFE34AF8E3D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,7 +331,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,12 +377,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -405,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -417,7 +411,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -763,7 +756,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +806,7 @@
       <c r="A3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C3" t="s">
@@ -856,15 +849,73 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="C6" s="7"/>
-      <c r="I6" s="8"/>
+      <c r="A5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
@@ -997,75 +1048,6 @@
       </c>
       <c r="I18" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.32</v>
-      </c>
-      <c r="F19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.76</v>
-      </c>
-      <c r="F20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.61</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>